<commit_message>
change the readme and add a instructions on python file
</commit_message>
<xml_diff>
--- a/IdiomasAMT.xlsx
+++ b/IdiomasAMT.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wender.junior\Desktop\Projetos\Correção de texto AMT\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gustavo.pereira\Desktop\Automatic_Translate\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B12F3606-0D51-45A4-81DA-F2D332C10C3E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{556B6059-3D8B-4DC5-AE69-E5DB3219BD1F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="35265" yWindow="1800" windowWidth="17370" windowHeight="11385" xr2:uid="{11EFB70B-DA7D-4F52-9231-78A572BB72FD}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{11EFB70B-DA7D-4F52-9231-78A572BB72FD}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1048" uniqueCount="327">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1007" uniqueCount="301">
   <si>
     <t>CODIGOITEMMENU</t>
   </si>
@@ -108,156 +108,12 @@
     <t>tiempo de espera de retraso</t>
   </si>
   <si>
-    <t>Almacenamiento</t>
-  </si>
-  <si>
-    <t>Storage</t>
-  </si>
-  <si>
-    <t>Operación</t>
-  </si>
-  <si>
-    <t>Tipos de divergencias</t>
-  </si>
-  <si>
-    <t>Tipo de Acciones Para Ajustar Divergencias</t>
-  </si>
-  <si>
-    <t>Tipos de modos de transporte</t>
-  </si>
-  <si>
-    <t>Tipos de señales del IRS</t>
-  </si>
-  <si>
-    <t>Tipos de procesos</t>
-  </si>
-  <si>
-    <t>Tipos de especies</t>
-  </si>
-  <si>
-    <t>Tipos de Productos</t>
-  </si>
-  <si>
-    <t>Productos</t>
-  </si>
-  <si>
-    <t>Tipos de Acciones Para Los Planes de Almacenamiento</t>
-  </si>
-  <si>
-    <t>Tipos de eventos com productos almacenados</t>
-  </si>
-  <si>
-    <t>Cualificaciones de la ubicación de almacenamiento</t>
-  </si>
-  <si>
-    <t>Ubicaciones de Almacenamiento</t>
-  </si>
-  <si>
-    <t>Documentos Fiscales</t>
-  </si>
-  <si>
-    <t>Importación de Documentos Fiscales</t>
-  </si>
-  <si>
-    <t>Requisitos Estándar Para Procesos</t>
-  </si>
-  <si>
-    <t>Procesos</t>
-  </si>
-  <si>
-    <t>Planes de Almacenamiento</t>
-  </si>
-  <si>
-    <t>Process</t>
-  </si>
-  <si>
-    <t>Recepción de productos</t>
-  </si>
-  <si>
-    <t>Registros de movimiento</t>
-  </si>
-  <si>
-    <t>Autorizaciones de lanzamiento de productos</t>
-  </si>
-  <si>
-    <t>Salida Del Producto</t>
-  </si>
-  <si>
-    <t>Envío de Productos</t>
-  </si>
-  <si>
-    <t>Horario de embarque</t>
-  </si>
-  <si>
-    <t>Consultar posición de productos para envío</t>
-  </si>
-  <si>
-    <t>Visualización gráfica de ubicaciones de almacenamiento</t>
-  </si>
-  <si>
     <t>Registros Básicos</t>
   </si>
   <si>
     <t>Compañías</t>
   </si>
   <si>
-    <t>Países</t>
-  </si>
-  <si>
-    <t>Puertos</t>
-  </si>
-  <si>
-    <t>Terminales</t>
-  </si>
-  <si>
-    <t>Dársena</t>
-  </si>
-  <si>
-    <t>Cargadero</t>
-  </si>
-  <si>
-    <t>Equipamientos</t>
-  </si>
-  <si>
-    <t>Tipos de Equipos</t>
-  </si>
-  <si>
-    <t>Tipos de Tiempo de Inactividad del Equipo</t>
-  </si>
-  <si>
-    <t>Equipment stop type</t>
-  </si>
-  <si>
-    <t>Maintenance History Registration</t>
-  </si>
-  <si>
-    <t>Registro del Historial de Mantenimiento</t>
-  </si>
-  <si>
-    <t>Responsable de Mantenimiento</t>
-  </si>
-  <si>
-    <t>Mano de Obra</t>
-  </si>
-  <si>
-    <t>Buques</t>
-  </si>
-  <si>
-    <t>Shipowners</t>
-  </si>
-  <si>
-    <t>Bandera</t>
-  </si>
-  <si>
-    <t>Datos de importacion</t>
-  </si>
-  <si>
-    <t>Tipos de Barcos</t>
-  </si>
-  <si>
-    <t>Agencia Marítima</t>
-  </si>
-  <si>
     <t>Recurso de Movilización</t>
   </si>
   <si>
@@ -303,39 +159,9 @@
     <t>Ganga</t>
   </si>
   <si>
-    <t>Orden de Servicio</t>
-  </si>
-  <si>
-    <t>Entrada de Trabajo Independiente</t>
-  </si>
-  <si>
-    <t>Entrada de trabalho separada</t>
-  </si>
-  <si>
-    <t>Appropriation of Resources</t>
-  </si>
-  <si>
-    <t>Embarque / Aterrizaje</t>
-  </si>
-  <si>
     <t>Financiero</t>
   </si>
   <si>
-    <t>La Seguridad</t>
-  </si>
-  <si>
-    <t>Administracion del Sistema</t>
-  </si>
-  <si>
-    <t>Flujo de Aprobación</t>
-  </si>
-  <si>
-    <t>Perfiles de Acceso al Sistema</t>
-  </si>
-  <si>
-    <t>Presupuesto de Oportunidad</t>
-  </si>
-  <si>
     <t>Nominaciones</t>
   </si>
   <si>
@@ -1015,6 +841,102 @@
   </si>
   <si>
     <t>Controle dos trens</t>
+  </si>
+  <si>
+    <t>Permissões especiais</t>
+  </si>
+  <si>
+    <t>Reabrir operações</t>
+  </si>
+  <si>
+    <t>Licença</t>
+  </si>
+  <si>
+    <t>Cadastro Nível Demora</t>
+  </si>
+  <si>
+    <t>Recurso de movilización</t>
+  </si>
+  <si>
+    <t>Deberes generales del trabajador</t>
+  </si>
+  <si>
+    <t>Apropiación de Recursos</t>
+  </si>
+  <si>
+    <t>Seguridad</t>
+  </si>
+  <si>
+    <t>De servicio</t>
+  </si>
+  <si>
+    <t>Aviso de E-mail</t>
+  </si>
+  <si>
+    <t>Administracion del sistema</t>
+  </si>
+  <si>
+    <t>Flujos de aprobación</t>
+  </si>
+  <si>
+    <t>Perfiles de acceso al sistema</t>
+  </si>
+  <si>
+    <t>Presupuesto de oportunidad</t>
+  </si>
+  <si>
+    <t>Atenciones</t>
+  </si>
+  <si>
+    <t>Planificación Anual de Operaciones</t>
+  </si>
+  <si>
+    <t>Gastos Generales de Naves</t>
+  </si>
+  <si>
+    <t>Suministros a Buques</t>
+  </si>
+  <si>
+    <t>Informe para Liberación de Notas de Débito</t>
+  </si>
+  <si>
+    <t>Colas de aprobación</t>
+  </si>
+  <si>
+    <t>Tipos de gastos de oportunidad</t>
+  </si>
+  <si>
+    <t>Tipos de gastos de envío</t>
+  </si>
+  <si>
+    <t>Tipos de horario</t>
+  </si>
+  <si>
+    <t>Tipos de Abastecimiento a Buques</t>
+  </si>
+  <si>
+    <t>Supervisores Laborales de Terceros</t>
+  </si>
+  <si>
+    <t>Third-Party Labor Supervisors</t>
+  </si>
+  <si>
+    <t>Practical</t>
+  </si>
+  <si>
+    <t>Empresas de empeño</t>
+  </si>
+  <si>
+    <t>Tablas de Precios</t>
+  </si>
+  <si>
+    <t>Parámetros de cálculo del presupuesto de oportunidad</t>
+  </si>
+  <si>
+    <t>Tablas de costos de almacenamiento</t>
+  </si>
+  <si>
+    <t>Tiempos estándar para la llegada del producto</t>
   </si>
 </sst>
 </file>
@@ -1173,7 +1095,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1186,9 +1108,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1220,7 +1139,7 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1571,8 +1490,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E558AFCB-78DF-44C5-B1D8-001C23AF9A87}">
   <dimension ref="A1:F349"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A148" workbookViewId="0">
-      <selection activeCell="C166" sqref="C166"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1:D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1592,39 +1511,39 @@
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>324</v>
+      <c r="D1" s="17" t="s">
+        <v>266</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>325</v>
+        <v>267</v>
       </c>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="1">
-        <v>1</v>
+        <v>400</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="D2" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>269</v>
+      </c>
+      <c r="D2" s="17" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" s="1">
-        <v>1</v>
+        <v>401</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C3" s="5" t="s">
-        <v>24</v>
+        <v>29</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>270</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>21</v>
@@ -1632,13 +1551,13 @@
     </row>
     <row r="4" spans="1:5">
       <c r="A4" s="1">
-        <v>2</v>
+        <v>394</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C4" s="5" t="s">
-        <v>26</v>
+        <v>29</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>271</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>21</v>
@@ -1646,13 +1565,13 @@
     </row>
     <row r="5" spans="1:5">
       <c r="A5" s="1">
-        <v>3</v>
+        <v>404</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C5" s="5" t="s">
-        <v>13</v>
+        <v>29</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>272</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>21</v>
@@ -1660,13 +1579,13 @@
     </row>
     <row r="6" spans="1:5">
       <c r="A6" s="1">
-        <v>4</v>
+        <v>72</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C6" s="5" t="s">
-        <v>27</v>
+      <c r="C6" s="1" t="s">
+        <v>273</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>21</v>
@@ -1674,13 +1593,13 @@
     </row>
     <row r="7" spans="1:5">
       <c r="A7" s="1">
-        <v>5</v>
+        <v>78</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C7" s="5" t="s">
-        <v>28</v>
+      <c r="C7" s="1" t="s">
+        <v>274</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>21</v>
@@ -1688,13 +1607,13 @@
     </row>
     <row r="8" spans="1:5">
       <c r="A8" s="1">
-        <v>6</v>
+        <v>82</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C8" s="5" t="s">
-        <v>29</v>
+      <c r="C8" s="1" t="s">
+        <v>275</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>21</v>
@@ -1702,13 +1621,13 @@
     </row>
     <row r="9" spans="1:5">
       <c r="A9" s="1">
-        <v>8</v>
+        <v>107</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C9" s="5" t="s">
-        <v>30</v>
+      <c r="C9" s="1" t="s">
+        <v>41</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>21</v>
@@ -1716,13 +1635,13 @@
     </row>
     <row r="10" spans="1:5">
       <c r="A10" s="1">
-        <v>9</v>
+        <v>108</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C10" s="5" t="s">
-        <v>31</v>
+      <c r="C10" s="1" t="s">
+        <v>276</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>21</v>
@@ -1730,13 +1649,13 @@
     </row>
     <row r="11" spans="1:5">
       <c r="A11" s="1">
-        <v>12</v>
+        <v>361</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>3</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>32</v>
+        <v>277</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>21</v>
@@ -1744,13 +1663,13 @@
     </row>
     <row r="12" spans="1:5">
       <c r="A12" s="1">
-        <v>13</v>
+        <v>374</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>3</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>33</v>
+        <v>278</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>21</v>
@@ -1758,13 +1677,13 @@
     </row>
     <row r="13" spans="1:5">
       <c r="A13" s="1">
-        <v>14</v>
+        <v>110</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>3</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>34</v>
+        <v>279</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>21</v>
@@ -1772,13 +1691,13 @@
     </row>
     <row r="14" spans="1:5">
       <c r="A14" s="1">
-        <v>16</v>
+        <v>111</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>3</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>35</v>
+        <v>4</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>21</v>
@@ -1786,13 +1705,13 @@
     </row>
     <row r="15" spans="1:5">
       <c r="A15" s="1">
-        <v>17</v>
+        <v>112</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>3</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>36</v>
+        <v>280</v>
       </c>
       <c r="D15" s="1" t="s">
         <v>21</v>
@@ -1800,13 +1719,13 @@
     </row>
     <row r="16" spans="1:5">
       <c r="A16" s="1">
-        <v>19</v>
+        <v>113</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>3</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>37</v>
+        <v>281</v>
       </c>
       <c r="D16" s="1" t="s">
         <v>21</v>
@@ -1814,13 +1733,13 @@
     </row>
     <row r="17" spans="1:4">
       <c r="A17" s="1">
-        <v>20</v>
+        <v>128</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>3</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>38</v>
+        <v>282</v>
       </c>
       <c r="D17" s="1" t="s">
         <v>21</v>
@@ -1828,13 +1747,13 @@
     </row>
     <row r="18" spans="1:4">
       <c r="A18" s="1">
-        <v>22</v>
+        <v>129</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>3</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="D18" s="1" t="s">
         <v>21</v>
@@ -1842,13 +1761,13 @@
     </row>
     <row r="19" spans="1:4">
       <c r="A19" s="1">
-        <v>23</v>
+        <v>130</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>3</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>40</v>
+        <v>283</v>
       </c>
       <c r="D19" s="1" t="s">
         <v>21</v>
@@ -1856,13 +1775,13 @@
     </row>
     <row r="20" spans="1:4">
       <c r="A20" s="1">
-        <v>24</v>
+        <v>131</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>3</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>41</v>
+        <v>284</v>
       </c>
       <c r="D20" s="1" t="s">
         <v>21</v>
@@ -1870,13 +1789,13 @@
     </row>
     <row r="21" spans="1:4">
       <c r="A21" s="1">
-        <v>25</v>
+        <v>132</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>3</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>42</v>
+        <v>285</v>
       </c>
       <c r="D21" s="1" t="s">
         <v>21</v>
@@ -1884,13 +1803,13 @@
     </row>
     <row r="22" spans="1:4">
       <c r="A22" s="1">
-        <v>25</v>
+        <v>133</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>12</v>
+        <v>3</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>44</v>
+        <v>286</v>
       </c>
       <c r="D22" s="1" t="s">
         <v>21</v>
@@ -1898,13 +1817,13 @@
     </row>
     <row r="23" spans="1:4">
       <c r="A23" s="1">
-        <v>26</v>
+        <v>134</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>3</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>43</v>
+        <v>287</v>
       </c>
       <c r="D23" s="1" t="s">
         <v>21</v>
@@ -1912,13 +1831,13 @@
     </row>
     <row r="24" spans="1:4">
       <c r="A24" s="1">
-        <v>27</v>
+        <v>135</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>3</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="D24" s="1" t="s">
         <v>21</v>
@@ -1926,13 +1845,13 @@
     </row>
     <row r="25" spans="1:4">
       <c r="A25" s="1">
-        <v>28</v>
+        <v>136</v>
       </c>
       <c r="B25" s="1" t="s">
         <v>3</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>46</v>
+        <v>288</v>
       </c>
       <c r="D25" s="1" t="s">
         <v>21</v>
@@ -1940,13 +1859,13 @@
     </row>
     <row r="26" spans="1:4">
       <c r="A26" s="1">
-        <v>29</v>
+        <v>137</v>
       </c>
       <c r="B26" s="1" t="s">
         <v>3</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>47</v>
+        <v>289</v>
       </c>
       <c r="D26" s="1" t="s">
         <v>21</v>
@@ -1954,13 +1873,13 @@
     </row>
     <row r="27" spans="1:4">
       <c r="A27" s="1">
-        <v>30</v>
+        <v>138</v>
       </c>
       <c r="B27" s="1" t="s">
         <v>3</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>48</v>
+        <v>290</v>
       </c>
       <c r="D27" s="1" t="s">
         <v>21</v>
@@ -1968,13 +1887,13 @@
     </row>
     <row r="28" spans="1:4">
       <c r="A28" s="1">
-        <v>31</v>
+        <v>140</v>
       </c>
       <c r="B28" s="1" t="s">
         <v>3</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="D28" s="1" t="s">
         <v>21</v>
@@ -1982,13 +1901,13 @@
     </row>
     <row r="29" spans="1:4">
       <c r="A29" s="1">
-        <v>32</v>
+        <v>141</v>
       </c>
       <c r="B29" s="1" t="s">
         <v>3</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>50</v>
+        <v>291</v>
       </c>
       <c r="D29" s="1" t="s">
         <v>21</v>
@@ -1996,13 +1915,13 @@
     </row>
     <row r="30" spans="1:4">
       <c r="A30" s="1">
-        <v>33</v>
+        <v>142</v>
       </c>
       <c r="B30" s="1" t="s">
         <v>3</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>51</v>
+        <v>292</v>
       </c>
       <c r="D30" s="1" t="s">
         <v>21</v>
@@ -2010,13 +1929,13 @@
     </row>
     <row r="31" spans="1:4">
       <c r="A31" s="1">
-        <v>35</v>
+        <v>144</v>
       </c>
       <c r="B31" s="1" t="s">
         <v>3</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="D31" s="1" t="s">
         <v>21</v>
@@ -2024,13 +1943,13 @@
     </row>
     <row r="32" spans="1:4">
       <c r="A32" s="1">
-        <v>37</v>
+        <v>145</v>
       </c>
       <c r="B32" s="1" t="s">
         <v>3</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>53</v>
+        <v>293</v>
       </c>
       <c r="D32" s="1" t="s">
         <v>21</v>
@@ -2038,13 +1957,13 @@
     </row>
     <row r="33" spans="1:4">
       <c r="A33" s="1">
-        <v>38</v>
+        <v>145</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>54</v>
+        <v>294</v>
       </c>
       <c r="D33" s="1" t="s">
         <v>21</v>
@@ -2052,13 +1971,13 @@
     </row>
     <row r="34" spans="1:4">
       <c r="A34" s="1">
-        <v>43</v>
+        <v>146</v>
       </c>
       <c r="B34" s="1" t="s">
         <v>3</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>55</v>
+        <v>295</v>
       </c>
       <c r="D34" s="1" t="s">
         <v>21</v>
@@ -2066,13 +1985,13 @@
     </row>
     <row r="35" spans="1:4">
       <c r="A35" s="1">
-        <v>45</v>
+        <v>147</v>
       </c>
       <c r="B35" s="1" t="s">
         <v>3</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>56</v>
+        <v>296</v>
       </c>
       <c r="D35" s="1" t="s">
         <v>21</v>
@@ -2080,13 +1999,13 @@
     </row>
     <row r="36" spans="1:4">
       <c r="A36" s="1">
-        <v>46</v>
+        <v>148</v>
       </c>
       <c r="B36" s="1" t="s">
         <v>3</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>56</v>
+        <v>297</v>
       </c>
       <c r="D36" s="1" t="s">
         <v>21</v>
@@ -2094,13 +2013,13 @@
     </row>
     <row r="37" spans="1:4">
       <c r="A37" s="1">
-        <v>47</v>
+        <v>149</v>
       </c>
       <c r="B37" s="1" t="s">
         <v>3</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>57</v>
+        <v>298</v>
       </c>
       <c r="D37" s="1" t="s">
         <v>21</v>
@@ -2108,13 +2027,13 @@
     </row>
     <row r="38" spans="1:4">
       <c r="A38" s="1">
-        <v>48</v>
+        <v>150</v>
       </c>
       <c r="B38" s="1" t="s">
         <v>3</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>59</v>
+        <v>299</v>
       </c>
       <c r="D38" s="1" t="s">
         <v>21</v>
@@ -2122,290 +2041,222 @@
     </row>
     <row r="39" spans="1:4">
       <c r="A39" s="1">
-        <v>49</v>
+        <v>157</v>
       </c>
       <c r="B39" s="1" t="s">
         <v>3</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>58</v>
+        <v>300</v>
       </c>
       <c r="D39" s="1" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="40" spans="1:4">
-      <c r="A40" s="1">
-        <v>50</v>
-      </c>
+      <c r="A40" s="1"/>
       <c r="B40" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C40" s="1" t="s">
-        <v>60</v>
-      </c>
+      <c r="C40" s="1"/>
       <c r="D40" s="1" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="41" spans="1:4">
-      <c r="A41" s="1">
-        <v>51</v>
-      </c>
+      <c r="A41" s="1"/>
       <c r="B41" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C41" s="1" t="s">
-        <v>60</v>
-      </c>
+      <c r="C41" s="1"/>
       <c r="D41" s="1" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="42" spans="1:4">
-      <c r="A42" s="1">
-        <v>52</v>
-      </c>
+      <c r="A42" s="1"/>
       <c r="B42" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C42" s="1" t="s">
-        <v>61</v>
-      </c>
+      <c r="C42" s="1"/>
       <c r="D42" s="1" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="43" spans="1:4">
-      <c r="A43" s="1">
-        <v>53</v>
-      </c>
+      <c r="A43" s="1"/>
       <c r="B43" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C43" s="1" t="s">
-        <v>62</v>
-      </c>
+      <c r="C43" s="1"/>
       <c r="D43" s="1" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="44" spans="1:4">
-      <c r="A44" s="1">
-        <v>53</v>
-      </c>
+      <c r="A44" s="1"/>
       <c r="B44" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C44" s="1" t="s">
-        <v>63</v>
-      </c>
+        <v>3</v>
+      </c>
+      <c r="C44" s="1"/>
       <c r="D44" s="1" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="45" spans="1:4">
-      <c r="A45" s="1">
-        <v>54</v>
-      </c>
+      <c r="A45" s="1"/>
       <c r="B45" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C45" s="1" t="s">
-        <v>65</v>
-      </c>
+      <c r="C45" s="1"/>
       <c r="D45" s="1" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="46" spans="1:4">
-      <c r="A46" s="1">
-        <v>54</v>
-      </c>
+      <c r="A46" s="1"/>
       <c r="B46" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C46" s="1" t="s">
-        <v>64</v>
-      </c>
+        <v>3</v>
+      </c>
+      <c r="C46" s="1"/>
       <c r="D46" s="1" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="47" spans="1:4">
-      <c r="A47" s="1">
-        <v>55</v>
-      </c>
+      <c r="A47" s="1"/>
       <c r="B47" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C47" s="1" t="s">
+      <c r="C47" s="1"/>
+      <c r="D47" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4">
+      <c r="A48" s="1"/>
+      <c r="B48" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C48" s="1"/>
+      <c r="D48" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6">
+      <c r="A49" s="1"/>
+      <c r="B49" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C49" s="1"/>
+      <c r="D49" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6">
+      <c r="A50" s="1"/>
+      <c r="B50" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C50" s="1"/>
+      <c r="D50" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6">
+      <c r="A51" s="1"/>
+      <c r="B51" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C51" s="1"/>
+      <c r="D51" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6">
+      <c r="A52" s="1"/>
+      <c r="B52" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C52" s="1"/>
+      <c r="D52" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6">
+      <c r="A53" s="1"/>
+      <c r="B53" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C53" s="1"/>
+      <c r="D53" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6">
+      <c r="A54" s="1"/>
+      <c r="B54" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C54" s="1"/>
+      <c r="D54" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6">
+      <c r="A55" s="1"/>
+      <c r="B55" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C55" s="1"/>
+      <c r="D55" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" ht="15.75" thickBot="1">
+      <c r="A56" s="1"/>
+      <c r="B56" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C56" s="1"/>
+      <c r="D56" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" ht="23.25">
+      <c r="A57" s="6">
         <v>66</v>
       </c>
-      <c r="D47" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4">
-      <c r="A48" s="1">
-        <v>56</v>
-      </c>
-      <c r="B48" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C48" s="1" t="s">
+      <c r="B57" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="C57" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="D57" s="7"/>
+      <c r="E57" s="15" t="s">
+        <v>36</v>
+      </c>
+      <c r="F57" s="8" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" ht="24" thickBot="1">
+      <c r="A58" s="9">
         <v>67</v>
       </c>
-      <c r="D48" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="49" spans="1:6">
-      <c r="A49" s="1">
-        <v>57</v>
-      </c>
-      <c r="B49" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C49" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="D49" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="50" spans="1:6">
-      <c r="A50" s="1">
-        <v>58</v>
-      </c>
-      <c r="B50" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C50" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="D50" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="51" spans="1:6">
-      <c r="A51" s="1">
-        <v>59</v>
-      </c>
-      <c r="B51" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C51" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="D51" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="52" spans="1:6">
-      <c r="A52" s="1">
-        <v>60</v>
-      </c>
-      <c r="B52" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C52" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="D52" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="53" spans="1:6">
-      <c r="A53" s="1">
-        <v>61</v>
-      </c>
-      <c r="B53" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C53" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="D53" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="54" spans="1:6">
-      <c r="A54" s="1">
-        <v>62</v>
-      </c>
-      <c r="B54" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C54" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="D54" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="55" spans="1:6">
-      <c r="A55" s="1">
-        <v>63</v>
-      </c>
-      <c r="B55" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C55" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="D55" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="56" spans="1:6" ht="15.75" thickBot="1">
-      <c r="A56" s="1">
-        <v>64</v>
-      </c>
-      <c r="B56" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C56" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="D56" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="57" spans="1:6" ht="23.25">
-      <c r="A57" s="7">
-        <v>66</v>
-      </c>
-      <c r="B57" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="C57" s="8" t="s">
-        <v>79</v>
-      </c>
-      <c r="D57" s="8"/>
-      <c r="E57" s="16" t="s">
-        <v>84</v>
-      </c>
-      <c r="F57" s="9" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="58" spans="1:6" ht="24" thickBot="1">
-      <c r="A58" s="10">
-        <v>67</v>
-      </c>
-      <c r="B58" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="C58" s="6" t="s">
-        <v>79</v>
-      </c>
-      <c r="D58" s="6"/>
-      <c r="E58" s="17" t="s">
-        <v>84</v>
-      </c>
-      <c r="F58" s="11" t="s">
-        <v>85</v>
+      <c r="B58" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C58" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="D58" s="5"/>
+      <c r="E58" s="16" t="s">
+        <v>36</v>
+      </c>
+      <c r="F58" s="10" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="59" spans="1:6">
@@ -2416,7 +2267,7 @@
         <v>3</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>74</v>
+        <v>26</v>
       </c>
       <c r="D59" s="1" t="s">
         <v>21</v>
@@ -2430,7 +2281,7 @@
         <v>3</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>75</v>
+        <v>27</v>
       </c>
       <c r="D60" s="1" t="s">
         <v>21</v>
@@ -2444,7 +2295,7 @@
         <v>3</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>76</v>
+        <v>28</v>
       </c>
       <c r="D61" s="1" t="s">
         <v>21</v>
@@ -2458,7 +2309,7 @@
         <v>3</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>78</v>
+        <v>30</v>
       </c>
       <c r="D62" s="1" t="s">
         <v>21</v>
@@ -2472,10 +2323,10 @@
         <v>3</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>80</v>
+        <v>32</v>
       </c>
       <c r="D63" s="1" t="s">
-        <v>82</v>
+        <v>34</v>
       </c>
     </row>
     <row r="64" spans="1:6">
@@ -2483,13 +2334,13 @@
         <v>76</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>77</v>
+        <v>29</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>81</v>
+        <v>33</v>
       </c>
       <c r="D64" s="1" t="s">
-        <v>82</v>
+        <v>34</v>
       </c>
     </row>
     <row r="65" spans="1:5">
@@ -2500,10 +2351,10 @@
         <v>3</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>87</v>
+        <v>39</v>
       </c>
       <c r="D65" s="1" t="s">
-        <v>82</v>
+        <v>34</v>
       </c>
     </row>
     <row r="66" spans="1:5">
@@ -2511,13 +2362,13 @@
         <v>77</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>77</v>
+        <v>29</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>83</v>
+        <v>35</v>
       </c>
       <c r="D66" s="1" t="s">
-        <v>82</v>
+        <v>34</v>
       </c>
     </row>
     <row r="67" spans="1:5" ht="15.75" thickBot="1">
@@ -2528,191 +2379,119 @@
         <v>3</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>86</v>
+        <v>38</v>
       </c>
       <c r="D67" s="1" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="68" spans="1:5" ht="24" thickBot="1">
-      <c r="A68" s="12">
+      <c r="A68" s="11">
         <v>79</v>
       </c>
-      <c r="B68" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="C68" s="13" t="s">
-        <v>88</v>
-      </c>
-      <c r="D68" s="14"/>
-      <c r="E68" s="15" t="s">
-        <v>84</v>
+      <c r="B68" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="C68" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="D68" s="13"/>
+      <c r="E68" s="14" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="69" spans="1:5">
-      <c r="A69" s="1">
-        <v>80</v>
-      </c>
-      <c r="B69" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C69" s="1" t="s">
-        <v>89</v>
-      </c>
+      <c r="A69" s="1"/>
+      <c r="B69" s="1"/>
+      <c r="C69" s="1"/>
       <c r="D69" s="1" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="70" spans="1:5">
-      <c r="A70" s="18">
-        <v>81</v>
-      </c>
-      <c r="B70" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C70" s="1" t="s">
-        <v>90</v>
-      </c>
+      <c r="A70" s="1"/>
+      <c r="B70" s="1"/>
+      <c r="C70" s="1"/>
       <c r="D70" s="1" t="s">
-        <v>82</v>
+        <v>34</v>
       </c>
     </row>
     <row r="71" spans="1:5">
-      <c r="A71" s="18">
-        <v>81</v>
-      </c>
-      <c r="B71" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="C71" s="1" t="s">
-        <v>91</v>
-      </c>
+      <c r="A71" s="1"/>
+      <c r="B71" s="1"/>
+      <c r="C71" s="1"/>
       <c r="D71" s="1" t="s">
-        <v>82</v>
+        <v>34</v>
       </c>
     </row>
     <row r="72" spans="1:5">
-      <c r="A72" s="18">
-        <v>82</v>
-      </c>
-      <c r="B72" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C72" s="1" t="s">
-        <v>92</v>
-      </c>
+      <c r="A72" s="1"/>
+      <c r="B72" s="1"/>
+      <c r="C72" s="1"/>
       <c r="D72" s="1" t="s">
-        <v>82</v>
+        <v>34</v>
       </c>
     </row>
     <row r="73" spans="1:5">
-      <c r="A73" s="18">
-        <v>84</v>
-      </c>
-      <c r="B73" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C73" s="1" t="s">
-        <v>93</v>
-      </c>
+      <c r="A73" s="1"/>
+      <c r="B73" s="1"/>
+      <c r="C73" s="1"/>
       <c r="D73" s="1" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="74" spans="1:5">
-      <c r="A74" s="18">
-        <v>107</v>
-      </c>
-      <c r="B74" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C74" s="1" t="s">
-        <v>94</v>
-      </c>
+      <c r="A74" s="1"/>
+      <c r="B74" s="1"/>
+      <c r="C74" s="1"/>
       <c r="D74" s="1" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="75" spans="1:5">
-      <c r="A75" s="18">
-        <v>108</v>
-      </c>
-      <c r="B75" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C75" s="1" t="s">
-        <v>95</v>
-      </c>
+      <c r="A75" s="1"/>
+      <c r="B75" s="1"/>
+      <c r="C75" s="1"/>
       <c r="D75" s="1" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="76" spans="1:5">
-      <c r="A76" s="18">
-        <v>110</v>
-      </c>
-      <c r="B76" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C76" s="1" t="s">
-        <v>96</v>
-      </c>
+      <c r="A76" s="1"/>
+      <c r="B76" s="1"/>
+      <c r="C76" s="1"/>
       <c r="D76" s="1" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="77" spans="1:5">
-      <c r="A77" s="1">
-        <v>111</v>
-      </c>
-      <c r="B77" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C77" s="1" t="s">
-        <v>4</v>
-      </c>
+      <c r="A77" s="1"/>
+      <c r="B77" s="1"/>
+      <c r="C77" s="1"/>
       <c r="D77" s="1" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="78" spans="1:5">
-      <c r="A78" s="1">
-        <v>112</v>
-      </c>
-      <c r="B78" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C78" s="1" t="s">
-        <v>97</v>
-      </c>
+      <c r="A78" s="1"/>
+      <c r="B78" s="1"/>
+      <c r="C78" s="1"/>
       <c r="D78" s="1" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="79" spans="1:5">
-      <c r="A79" s="1">
-        <v>113</v>
-      </c>
-      <c r="B79" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C79" s="1" t="s">
-        <v>98</v>
-      </c>
+      <c r="A79" s="1"/>
+      <c r="B79" s="1"/>
+      <c r="C79" s="1"/>
       <c r="D79" s="1" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="80" spans="1:5">
-      <c r="A80" s="1">
-        <v>128</v>
-      </c>
-      <c r="B80" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C80" s="1" t="s">
-        <v>99</v>
-      </c>
+      <c r="A80" s="1"/>
+      <c r="B80" s="1"/>
+      <c r="C80" s="1"/>
       <c r="D80" s="1" t="s">
         <v>21</v>
       </c>
@@ -2725,7 +2504,7 @@
         <v>3</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>100</v>
+        <v>42</v>
       </c>
       <c r="D81" s="1" t="s">
         <v>21</v>
@@ -2739,7 +2518,7 @@
         <v>3</v>
       </c>
       <c r="C82" s="1" t="s">
-        <v>101</v>
+        <v>43</v>
       </c>
       <c r="D82" s="1" t="s">
         <v>21</v>
@@ -2753,7 +2532,7 @@
         <v>3</v>
       </c>
       <c r="C83" s="1" t="s">
-        <v>102</v>
+        <v>44</v>
       </c>
       <c r="D83" s="1" t="s">
         <v>21</v>
@@ -2767,7 +2546,7 @@
         <v>3</v>
       </c>
       <c r="C84" s="1" t="s">
-        <v>103</v>
+        <v>45</v>
       </c>
       <c r="D84" s="1" t="s">
         <v>21</v>
@@ -2795,7 +2574,7 @@
         <v>3</v>
       </c>
       <c r="C86" s="1" t="s">
-        <v>104</v>
+        <v>46</v>
       </c>
       <c r="D86" s="1" t="s">
         <v>21</v>
@@ -2809,7 +2588,7 @@
         <v>3</v>
       </c>
       <c r="C87" s="1" t="s">
-        <v>105</v>
+        <v>47</v>
       </c>
       <c r="D87" s="1" t="s">
         <v>21</v>
@@ -2823,7 +2602,7 @@
         <v>3</v>
       </c>
       <c r="C88" s="1" t="s">
-        <v>106</v>
+        <v>48</v>
       </c>
       <c r="D88" s="1" t="s">
         <v>21</v>
@@ -2837,7 +2616,7 @@
         <v>3</v>
       </c>
       <c r="C89" s="1" t="s">
-        <v>107</v>
+        <v>49</v>
       </c>
       <c r="D89" s="1" t="s">
         <v>21</v>
@@ -2851,7 +2630,7 @@
         <v>3</v>
       </c>
       <c r="C90" s="1" t="s">
-        <v>108</v>
+        <v>50</v>
       </c>
       <c r="D90" s="1" t="s">
         <v>21</v>
@@ -2865,7 +2644,7 @@
         <v>3</v>
       </c>
       <c r="C91" s="1" t="s">
-        <v>109</v>
+        <v>51</v>
       </c>
       <c r="D91" s="1" t="s">
         <v>21</v>
@@ -2879,7 +2658,7 @@
         <v>3</v>
       </c>
       <c r="C92" s="1" t="s">
-        <v>110</v>
+        <v>52</v>
       </c>
       <c r="D92" s="1" t="s">
         <v>21</v>
@@ -2893,7 +2672,7 @@
         <v>3</v>
       </c>
       <c r="C93" s="1" t="s">
-        <v>111</v>
+        <v>53</v>
       </c>
       <c r="D93" s="1" t="s">
         <v>21</v>
@@ -2907,7 +2686,7 @@
         <v>3</v>
       </c>
       <c r="C94" s="1" t="s">
-        <v>112</v>
+        <v>54</v>
       </c>
       <c r="D94" s="1" t="s">
         <v>21</v>
@@ -2935,7 +2714,7 @@
         <v>3</v>
       </c>
       <c r="C96" s="1" t="s">
-        <v>113</v>
+        <v>55</v>
       </c>
       <c r="D96" s="1" t="s">
         <v>21</v>
@@ -2949,7 +2728,7 @@
         <v>3</v>
       </c>
       <c r="C97" s="1" t="s">
-        <v>114</v>
+        <v>56</v>
       </c>
       <c r="D97" s="1" t="s">
         <v>21</v>
@@ -2963,7 +2742,7 @@
         <v>3</v>
       </c>
       <c r="C98" s="1" t="s">
-        <v>115</v>
+        <v>57</v>
       </c>
       <c r="D98" s="1" t="s">
         <v>21</v>
@@ -2977,7 +2756,7 @@
         <v>3</v>
       </c>
       <c r="C99" s="1" t="s">
-        <v>116</v>
+        <v>58</v>
       </c>
       <c r="D99" s="1" t="s">
         <v>21</v>
@@ -3047,7 +2826,7 @@
         <v>3</v>
       </c>
       <c r="C104" s="1" t="s">
-        <v>117</v>
+        <v>59</v>
       </c>
       <c r="D104" s="1" t="s">
         <v>21</v>
@@ -3075,7 +2854,7 @@
         <v>3</v>
       </c>
       <c r="C106" s="1" t="s">
-        <v>118</v>
+        <v>60</v>
       </c>
       <c r="D106" s="1" t="s">
         <v>21</v>
@@ -3103,7 +2882,7 @@
         <v>3</v>
       </c>
       <c r="C108" s="1" t="s">
-        <v>119</v>
+        <v>61</v>
       </c>
       <c r="D108" s="1" t="s">
         <v>21</v>
@@ -3117,7 +2896,7 @@
         <v>3</v>
       </c>
       <c r="C109" s="1" t="s">
-        <v>120</v>
+        <v>62</v>
       </c>
       <c r="D109" s="1" t="s">
         <v>21</v>
@@ -3131,7 +2910,7 @@
         <v>3</v>
       </c>
       <c r="C110" s="1" t="s">
-        <v>121</v>
+        <v>63</v>
       </c>
       <c r="D110" s="1" t="s">
         <v>21</v>
@@ -3159,7 +2938,7 @@
         <v>3</v>
       </c>
       <c r="C112" s="1" t="s">
-        <v>122</v>
+        <v>64</v>
       </c>
       <c r="D112" s="1" t="s">
         <v>21</v>
@@ -3187,7 +2966,7 @@
         <v>3</v>
       </c>
       <c r="C114" s="1" t="s">
-        <v>123</v>
+        <v>65</v>
       </c>
       <c r="D114" s="1" t="s">
         <v>21</v>
@@ -3215,7 +2994,7 @@
         <v>3</v>
       </c>
       <c r="C116" s="1" t="s">
-        <v>124</v>
+        <v>66</v>
       </c>
       <c r="D116" s="1" t="s">
         <v>21</v>
@@ -3257,7 +3036,7 @@
         <v>3</v>
       </c>
       <c r="C119" s="1" t="s">
-        <v>125</v>
+        <v>67</v>
       </c>
       <c r="D119" s="1" t="s">
         <v>21</v>
@@ -3271,7 +3050,7 @@
         <v>3</v>
       </c>
       <c r="C120" s="1" t="s">
-        <v>126</v>
+        <v>68</v>
       </c>
       <c r="D120" s="1" t="s">
         <v>21</v>
@@ -3285,7 +3064,7 @@
         <v>12</v>
       </c>
       <c r="C121" s="1" t="s">
-        <v>127</v>
+        <v>69</v>
       </c>
       <c r="D121" s="1" t="s">
         <v>21</v>
@@ -3299,7 +3078,7 @@
         <v>3</v>
       </c>
       <c r="C122" s="1" t="s">
-        <v>128</v>
+        <v>70</v>
       </c>
       <c r="D122" s="1" t="s">
         <v>21</v>
@@ -3313,7 +3092,7 @@
         <v>3</v>
       </c>
       <c r="C123" s="1" t="s">
-        <v>129</v>
+        <v>71</v>
       </c>
       <c r="D123" s="1" t="s">
         <v>21</v>
@@ -3327,7 +3106,7 @@
         <v>12</v>
       </c>
       <c r="C124" s="1" t="s">
-        <v>130</v>
+        <v>72</v>
       </c>
       <c r="D124" s="1" t="s">
         <v>21</v>
@@ -3341,7 +3120,7 @@
         <v>3</v>
       </c>
       <c r="C125" s="1" t="s">
-        <v>131</v>
+        <v>73</v>
       </c>
       <c r="D125" s="1" t="s">
         <v>21</v>
@@ -3355,7 +3134,7 @@
         <v>3</v>
       </c>
       <c r="C126" s="1" t="s">
-        <v>132</v>
+        <v>74</v>
       </c>
       <c r="D126" s="1" t="s">
         <v>21</v>
@@ -3369,7 +3148,7 @@
         <v>3</v>
       </c>
       <c r="C127" s="1" t="s">
-        <v>133</v>
+        <v>75</v>
       </c>
       <c r="D127" s="1" t="s">
         <v>21</v>
@@ -3383,7 +3162,7 @@
         <v>12</v>
       </c>
       <c r="C128" s="1" t="s">
-        <v>134</v>
+        <v>76</v>
       </c>
       <c r="D128" s="1" t="s">
         <v>21</v>
@@ -3397,7 +3176,7 @@
         <v>3</v>
       </c>
       <c r="C129" s="1" t="s">
-        <v>136</v>
+        <v>78</v>
       </c>
       <c r="D129" s="1" t="s">
         <v>21</v>
@@ -3411,7 +3190,7 @@
         <v>12</v>
       </c>
       <c r="C130" s="1" t="s">
-        <v>135</v>
+        <v>77</v>
       </c>
       <c r="D130" s="1" t="s">
         <v>21</v>
@@ -3425,7 +3204,7 @@
         <v>3</v>
       </c>
       <c r="C131" s="1" t="s">
-        <v>137</v>
+        <v>79</v>
       </c>
       <c r="D131" s="1" t="s">
         <v>21</v>
@@ -3439,7 +3218,7 @@
         <v>12</v>
       </c>
       <c r="C132" s="1" t="s">
-        <v>138</v>
+        <v>80</v>
       </c>
       <c r="D132" s="1" t="s">
         <v>21</v>
@@ -3453,7 +3232,7 @@
         <v>3</v>
       </c>
       <c r="C133" s="1" t="s">
-        <v>139</v>
+        <v>81</v>
       </c>
       <c r="D133" s="1" t="s">
         <v>21</v>
@@ -3467,7 +3246,7 @@
         <v>3</v>
       </c>
       <c r="C134" s="1" t="s">
-        <v>140</v>
+        <v>82</v>
       </c>
       <c r="D134" s="1" t="s">
         <v>21</v>
@@ -3481,7 +3260,7 @@
         <v>12</v>
       </c>
       <c r="C135" s="1" t="s">
-        <v>141</v>
+        <v>83</v>
       </c>
       <c r="D135" s="1" t="s">
         <v>21</v>
@@ -3495,137 +3274,137 @@
         <v>3</v>
       </c>
       <c r="C136" s="1" t="s">
-        <v>142</v>
+        <v>84</v>
       </c>
       <c r="D136" s="1" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="137" spans="1:5" ht="24" thickBot="1">
-      <c r="A137" s="7">
+      <c r="A137" s="6">
         <v>195</v>
       </c>
-      <c r="B137" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="C137" s="8" t="s">
-        <v>143</v>
-      </c>
-      <c r="D137" s="8"/>
-      <c r="E137" s="15" t="s">
-        <v>84</v>
+      <c r="B137" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="C137" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="D137" s="7"/>
+      <c r="E137" s="14" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="138" spans="1:5" ht="24" thickBot="1">
-      <c r="A138" s="10">
+      <c r="A138" s="9">
         <v>195</v>
       </c>
-      <c r="B138" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="C138" s="6" t="s">
-        <v>143</v>
-      </c>
-      <c r="D138" s="6"/>
-      <c r="E138" s="15" t="s">
-        <v>84</v>
+      <c r="B138" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C138" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="D138" s="5"/>
+      <c r="E138" s="14" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="139" spans="1:5">
-      <c r="A139" s="18">
+      <c r="A139" s="1">
         <v>196</v>
       </c>
-      <c r="B139" s="18" t="s">
-        <v>3</v>
-      </c>
-      <c r="C139" s="18" t="s">
-        <v>144</v>
-      </c>
-      <c r="D139" s="18" t="s">
+      <c r="B139" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C139" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="D139" s="1" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="140" spans="1:5">
-      <c r="A140" s="18">
+      <c r="A140" s="1">
         <v>201</v>
       </c>
-      <c r="B140" s="18" t="s">
-        <v>3</v>
-      </c>
-      <c r="C140" s="18" t="s">
-        <v>145</v>
-      </c>
-      <c r="D140" s="18" t="s">
+      <c r="B140" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C140" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="D140" s="1" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="141" spans="1:5">
-      <c r="A141" s="18">
+      <c r="A141" s="1">
         <v>203</v>
       </c>
-      <c r="B141" s="18" t="s">
-        <v>3</v>
-      </c>
-      <c r="C141" s="18" t="s">
-        <v>146</v>
-      </c>
-      <c r="D141" s="18" t="s">
+      <c r="B141" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C141" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="D141" s="1" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="142" spans="1:5">
-      <c r="A142" s="18">
+      <c r="A142" s="1">
         <v>204</v>
       </c>
-      <c r="B142" s="18" t="s">
-        <v>3</v>
-      </c>
-      <c r="C142" s="18" t="s">
-        <v>147</v>
-      </c>
-      <c r="D142" s="18" t="s">
+      <c r="B142" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C142" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="D142" s="1" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="143" spans="1:5">
-      <c r="A143" s="18">
+      <c r="A143" s="1">
         <v>204</v>
       </c>
-      <c r="B143" s="18" t="s">
-        <v>12</v>
-      </c>
-      <c r="C143" s="18" t="s">
-        <v>148</v>
-      </c>
-      <c r="D143" s="18" t="s">
+      <c r="B143" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C143" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="D143" s="1" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="144" spans="1:5">
-      <c r="A144" s="18">
+      <c r="A144" s="1">
         <v>208</v>
       </c>
-      <c r="B144" s="18" t="s">
-        <v>3</v>
-      </c>
-      <c r="C144" s="18" t="s">
-        <v>149</v>
-      </c>
-      <c r="D144" s="18" t="s">
+      <c r="B144" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C144" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="D144" s="1" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="145" spans="1:4">
-      <c r="A145" s="18">
+      <c r="A145" s="1">
         <v>217</v>
       </c>
-      <c r="B145" s="18" t="s">
-        <v>3</v>
-      </c>
-      <c r="C145" s="18" t="s">
-        <v>150</v>
-      </c>
-      <c r="D145" s="18" t="s">
+      <c r="B145" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C145" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="D145" s="1" t="s">
         <v>21</v>
       </c>
     </row>
@@ -3650,8 +3429,8 @@
       <c r="B147" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C147" s="18" t="s">
-        <v>151</v>
+      <c r="C147" s="1" t="s">
+        <v>93</v>
       </c>
       <c r="D147" s="1" t="s">
         <v>21</v>
@@ -3664,8 +3443,8 @@
       <c r="B148" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C148" s="18" t="s">
-        <v>152</v>
+      <c r="C148" s="1" t="s">
+        <v>94</v>
       </c>
       <c r="D148" s="1" t="s">
         <v>21</v>
@@ -3678,8 +3457,8 @@
       <c r="B149" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C149" s="18" t="s">
-        <v>153</v>
+      <c r="C149" s="1" t="s">
+        <v>95</v>
       </c>
       <c r="D149" s="1" t="s">
         <v>21</v>
@@ -3692,8 +3471,8 @@
       <c r="B150" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C150" s="18" t="s">
-        <v>154</v>
+      <c r="C150" s="1" t="s">
+        <v>96</v>
       </c>
       <c r="D150" s="1" t="s">
         <v>21</v>
@@ -3706,8 +3485,8 @@
       <c r="B151" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C151" s="18" t="s">
-        <v>155</v>
+      <c r="C151" s="1" t="s">
+        <v>97</v>
       </c>
       <c r="D151" s="1" t="s">
         <v>21</v>
@@ -3763,7 +3542,7 @@
         <v>3</v>
       </c>
       <c r="C155" s="1" t="s">
-        <v>156</v>
+        <v>98</v>
       </c>
       <c r="D155" s="4" t="s">
         <v>21</v>
@@ -3777,7 +3556,7 @@
         <v>3</v>
       </c>
       <c r="C156" s="1" t="s">
-        <v>157</v>
+        <v>99</v>
       </c>
       <c r="D156" s="1" t="s">
         <v>21</v>
@@ -3791,7 +3570,7 @@
         <v>3</v>
       </c>
       <c r="C157" s="1" t="s">
-        <v>158</v>
+        <v>100</v>
       </c>
       <c r="D157" s="1" t="s">
         <v>21</v>
@@ -3805,7 +3584,7 @@
         <v>3</v>
       </c>
       <c r="C158" s="1" t="s">
-        <v>159</v>
+        <v>101</v>
       </c>
       <c r="D158" s="1" t="s">
         <v>21</v>
@@ -3819,7 +3598,7 @@
         <v>3</v>
       </c>
       <c r="C159" s="1" t="s">
-        <v>160</v>
+        <v>102</v>
       </c>
       <c r="D159" s="1" t="s">
         <v>21</v>
@@ -3833,7 +3612,7 @@
         <v>3</v>
       </c>
       <c r="C160" s="1" t="s">
-        <v>161</v>
+        <v>103</v>
       </c>
       <c r="D160" s="1" t="s">
         <v>21</v>
@@ -3847,7 +3626,7 @@
         <v>3</v>
       </c>
       <c r="C161" s="1" t="s">
-        <v>162</v>
+        <v>104</v>
       </c>
       <c r="D161" s="1" t="s">
         <v>21</v>
@@ -3861,7 +3640,7 @@
         <v>12</v>
       </c>
       <c r="C162" s="1" t="s">
-        <v>163</v>
+        <v>105</v>
       </c>
       <c r="D162" s="1" t="s">
         <v>21</v>
@@ -3875,7 +3654,7 @@
         <v>3</v>
       </c>
       <c r="C163" s="1" t="s">
-        <v>128</v>
+        <v>70</v>
       </c>
       <c r="D163" s="1" t="s">
         <v>21</v>
@@ -3889,7 +3668,7 @@
         <v>3</v>
       </c>
       <c r="C164" s="1" t="s">
-        <v>164</v>
+        <v>106</v>
       </c>
       <c r="D164" s="1" t="s">
         <v>21</v>
@@ -3917,7 +3696,7 @@
         <v>3</v>
       </c>
       <c r="C166" s="1" t="s">
-        <v>165</v>
+        <v>107</v>
       </c>
       <c r="D166" s="1" t="s">
         <v>21</v>
@@ -3931,7 +3710,7 @@
         <v>3</v>
       </c>
       <c r="C167" s="1" t="s">
-        <v>166</v>
+        <v>108</v>
       </c>
       <c r="D167" s="1" t="s">
         <v>21</v>
@@ -3942,10 +3721,10 @@
         <v>241</v>
       </c>
       <c r="B168" s="1" t="s">
-        <v>77</v>
+        <v>29</v>
       </c>
       <c r="C168" s="1" t="s">
-        <v>326</v>
+        <v>268</v>
       </c>
       <c r="D168" s="1" t="s">
         <v>21</v>
@@ -3973,7 +3752,7 @@
         <v>12</v>
       </c>
       <c r="C170" s="1" t="s">
-        <v>167</v>
+        <v>109</v>
       </c>
       <c r="D170" s="1" t="s">
         <v>21</v>
@@ -3984,10 +3763,10 @@
         <v>243</v>
       </c>
       <c r="B171" s="1" t="s">
-        <v>77</v>
+        <v>29</v>
       </c>
       <c r="C171" s="1" t="s">
-        <v>168</v>
+        <v>110</v>
       </c>
       <c r="D171" s="1" t="s">
         <v>21</v>
@@ -4001,7 +3780,7 @@
         <v>3</v>
       </c>
       <c r="C172" s="1" t="s">
-        <v>169</v>
+        <v>111</v>
       </c>
       <c r="D172" s="1" t="s">
         <v>21</v>
@@ -4015,7 +3794,7 @@
         <v>12</v>
       </c>
       <c r="C173" s="1" t="s">
-        <v>170</v>
+        <v>112</v>
       </c>
       <c r="D173" s="1" t="s">
         <v>21</v>
@@ -4029,7 +3808,7 @@
         <v>3</v>
       </c>
       <c r="C174" s="1" t="s">
-        <v>172</v>
+        <v>114</v>
       </c>
       <c r="D174" s="1" t="s">
         <v>21</v>
@@ -4043,7 +3822,7 @@
         <v>12</v>
       </c>
       <c r="C175" s="1" t="s">
-        <v>171</v>
+        <v>113</v>
       </c>
       <c r="D175" s="1" t="s">
         <v>21</v>
@@ -4057,7 +3836,7 @@
         <v>12</v>
       </c>
       <c r="C176" s="1" t="s">
-        <v>173</v>
+        <v>115</v>
       </c>
       <c r="D176" s="1" t="s">
         <v>21</v>
@@ -4071,7 +3850,7 @@
         <v>3</v>
       </c>
       <c r="C177" s="1" t="s">
-        <v>174</v>
+        <v>116</v>
       </c>
       <c r="D177" s="1" t="s">
         <v>21</v>
@@ -4085,7 +3864,7 @@
         <v>3</v>
       </c>
       <c r="C178" s="1" t="s">
-        <v>175</v>
+        <v>117</v>
       </c>
       <c r="D178" s="1" t="s">
         <v>21</v>
@@ -4099,7 +3878,7 @@
         <v>12</v>
       </c>
       <c r="C179" s="1" t="s">
-        <v>176</v>
+        <v>118</v>
       </c>
       <c r="D179" s="1" t="s">
         <v>21</v>
@@ -4113,7 +3892,7 @@
         <v>3</v>
       </c>
       <c r="C180" s="1" t="s">
-        <v>177</v>
+        <v>119</v>
       </c>
       <c r="D180" s="1" t="s">
         <v>21</v>
@@ -4127,7 +3906,7 @@
         <v>3</v>
       </c>
       <c r="C181" s="1" t="s">
-        <v>178</v>
+        <v>120</v>
       </c>
       <c r="D181" s="1" t="s">
         <v>21</v>
@@ -4155,7 +3934,7 @@
         <v>12</v>
       </c>
       <c r="C183" s="1" t="s">
-        <v>179</v>
+        <v>121</v>
       </c>
       <c r="D183" s="1" t="s">
         <v>21</v>
@@ -4169,7 +3948,7 @@
         <v>3</v>
       </c>
       <c r="C184" s="1" t="s">
-        <v>175</v>
+        <v>117</v>
       </c>
       <c r="D184" s="1" t="s">
         <v>21</v>
@@ -4183,7 +3962,7 @@
         <v>3</v>
       </c>
       <c r="C185" s="1" t="s">
-        <v>180</v>
+        <v>122</v>
       </c>
       <c r="D185" s="1" t="s">
         <v>21</v>
@@ -4197,7 +3976,7 @@
         <v>12</v>
       </c>
       <c r="C186" s="1" t="s">
-        <v>181</v>
+        <v>123</v>
       </c>
       <c r="D186" s="1" t="s">
         <v>21</v>
@@ -4225,7 +4004,7 @@
         <v>12</v>
       </c>
       <c r="C188" s="1" t="s">
-        <v>182</v>
+        <v>124</v>
       </c>
       <c r="D188" s="1" t="s">
         <v>21</v>
@@ -4239,7 +4018,7 @@
         <v>3</v>
       </c>
       <c r="C189" s="1" t="s">
-        <v>183</v>
+        <v>125</v>
       </c>
       <c r="D189" s="1" t="s">
         <v>21</v>
@@ -4253,7 +4032,7 @@
         <v>3</v>
       </c>
       <c r="C190" s="1" t="s">
-        <v>184</v>
+        <v>126</v>
       </c>
       <c r="D190" s="1" t="s">
         <v>21</v>
@@ -4267,7 +4046,7 @@
         <v>3</v>
       </c>
       <c r="C191" s="1" t="s">
-        <v>185</v>
+        <v>127</v>
       </c>
       <c r="D191" s="1" t="s">
         <v>21</v>
@@ -4281,7 +4060,7 @@
         <v>3</v>
       </c>
       <c r="C192" s="1" t="s">
-        <v>186</v>
+        <v>128</v>
       </c>
       <c r="D192" s="1" t="s">
         <v>21</v>
@@ -4295,7 +4074,7 @@
         <v>12</v>
       </c>
       <c r="C193" s="1" t="s">
-        <v>187</v>
+        <v>129</v>
       </c>
       <c r="D193" s="1" t="s">
         <v>21</v>
@@ -4309,7 +4088,7 @@
         <v>3</v>
       </c>
       <c r="C194" s="1" t="s">
-        <v>189</v>
+        <v>131</v>
       </c>
       <c r="D194" s="1" t="s">
         <v>21</v>
@@ -4323,7 +4102,7 @@
         <v>12</v>
       </c>
       <c r="C195" s="1" t="s">
-        <v>188</v>
+        <v>130</v>
       </c>
       <c r="D195" s="1" t="s">
         <v>21</v>
@@ -4351,7 +4130,7 @@
         <v>3</v>
       </c>
       <c r="C197" s="1" t="s">
-        <v>190</v>
+        <v>132</v>
       </c>
       <c r="D197" s="1" t="s">
         <v>21</v>
@@ -4365,7 +4144,7 @@
         <v>12</v>
       </c>
       <c r="C198" s="1" t="s">
-        <v>191</v>
+        <v>133</v>
       </c>
       <c r="D198" s="1" t="s">
         <v>21</v>
@@ -4379,7 +4158,7 @@
         <v>3</v>
       </c>
       <c r="C199" s="1" t="s">
-        <v>192</v>
+        <v>134</v>
       </c>
       <c r="D199" s="1" t="s">
         <v>21</v>
@@ -4393,7 +4172,7 @@
         <v>3</v>
       </c>
       <c r="C200" s="1" t="s">
-        <v>193</v>
+        <v>135</v>
       </c>
       <c r="D200" s="1" t="s">
         <v>21</v>
@@ -4407,7 +4186,7 @@
         <v>3</v>
       </c>
       <c r="C201" s="1" t="s">
-        <v>194</v>
+        <v>136</v>
       </c>
       <c r="D201" s="1" t="s">
         <v>21</v>
@@ -4421,7 +4200,7 @@
         <v>3</v>
       </c>
       <c r="C202" s="1" t="s">
-        <v>195</v>
+        <v>137</v>
       </c>
       <c r="D202" s="1" t="s">
         <v>21</v>
@@ -4435,7 +4214,7 @@
         <v>3</v>
       </c>
       <c r="C203" s="1" t="s">
-        <v>196</v>
+        <v>138</v>
       </c>
       <c r="D203" s="1" t="s">
         <v>21</v>
@@ -4449,7 +4228,7 @@
         <v>12</v>
       </c>
       <c r="C204" s="1" t="s">
-        <v>197</v>
+        <v>139</v>
       </c>
       <c r="D204" s="1" t="s">
         <v>21</v>
@@ -4463,7 +4242,7 @@
         <v>3</v>
       </c>
       <c r="C205" s="1" t="s">
-        <v>199</v>
+        <v>141</v>
       </c>
       <c r="D205" s="1" t="s">
         <v>21</v>
@@ -4477,7 +4256,7 @@
         <v>12</v>
       </c>
       <c r="C206" s="1" t="s">
-        <v>198</v>
+        <v>140</v>
       </c>
       <c r="D206" s="1" t="s">
         <v>21</v>
@@ -4491,7 +4270,7 @@
         <v>3</v>
       </c>
       <c r="C207" s="1" t="s">
-        <v>200</v>
+        <v>142</v>
       </c>
       <c r="D207" s="1" t="s">
         <v>21</v>
@@ -4505,7 +4284,7 @@
         <v>3</v>
       </c>
       <c r="C208" s="1" t="s">
-        <v>201</v>
+        <v>143</v>
       </c>
       <c r="D208" s="1" t="s">
         <v>21</v>
@@ -4519,7 +4298,7 @@
         <v>3</v>
       </c>
       <c r="C209" s="1" t="s">
-        <v>202</v>
+        <v>144</v>
       </c>
       <c r="D209" s="1" t="s">
         <v>21</v>
@@ -4533,7 +4312,7 @@
         <v>3</v>
       </c>
       <c r="C210" s="1" t="s">
-        <v>203</v>
+        <v>145</v>
       </c>
       <c r="D210" s="1" t="s">
         <v>21</v>
@@ -4547,7 +4326,7 @@
         <v>3</v>
       </c>
       <c r="C211" s="1" t="s">
-        <v>204</v>
+        <v>146</v>
       </c>
       <c r="D211" s="1" t="s">
         <v>21</v>
@@ -4561,7 +4340,7 @@
         <v>3</v>
       </c>
       <c r="C212" s="1" t="s">
-        <v>205</v>
+        <v>147</v>
       </c>
       <c r="D212" s="1" t="s">
         <v>21</v>
@@ -4575,7 +4354,7 @@
         <v>3</v>
       </c>
       <c r="C213" s="1" t="s">
-        <v>206</v>
+        <v>148</v>
       </c>
       <c r="D213" s="1" t="s">
         <v>21</v>
@@ -4589,7 +4368,7 @@
         <v>3</v>
       </c>
       <c r="C214" s="1" t="s">
-        <v>207</v>
+        <v>149</v>
       </c>
       <c r="D214" s="1" t="s">
         <v>21</v>
@@ -4603,7 +4382,7 @@
         <v>3</v>
       </c>
       <c r="C215" s="1" t="s">
-        <v>208</v>
+        <v>150</v>
       </c>
       <c r="D215" s="1" t="s">
         <v>21</v>
@@ -4617,7 +4396,7 @@
         <v>3</v>
       </c>
       <c r="C216" s="1" t="s">
-        <v>209</v>
+        <v>151</v>
       </c>
       <c r="D216" s="1" t="s">
         <v>21</v>
@@ -4631,7 +4410,7 @@
         <v>3</v>
       </c>
       <c r="C217" s="1" t="s">
-        <v>210</v>
+        <v>152</v>
       </c>
       <c r="D217" s="1" t="s">
         <v>21</v>
@@ -4645,7 +4424,7 @@
         <v>3</v>
       </c>
       <c r="C218" s="1" t="s">
-        <v>211</v>
+        <v>153</v>
       </c>
       <c r="D218" s="1" t="s">
         <v>21</v>
@@ -4659,7 +4438,7 @@
         <v>3</v>
       </c>
       <c r="C219" s="1" t="s">
-        <v>212</v>
+        <v>154</v>
       </c>
       <c r="D219" s="1" t="s">
         <v>21</v>
@@ -4673,7 +4452,7 @@
         <v>3</v>
       </c>
       <c r="C220" s="1" t="s">
-        <v>213</v>
+        <v>155</v>
       </c>
       <c r="D220" s="1" t="s">
         <v>21</v>
@@ -4687,7 +4466,7 @@
         <v>3</v>
       </c>
       <c r="C221" s="1" t="s">
-        <v>215</v>
+        <v>157</v>
       </c>
       <c r="D221" s="1" t="s">
         <v>21</v>
@@ -4701,7 +4480,7 @@
         <v>12</v>
       </c>
       <c r="C222" s="1" t="s">
-        <v>216</v>
+        <v>158</v>
       </c>
       <c r="D222" s="1" t="s">
         <v>21</v>
@@ -4715,7 +4494,7 @@
         <v>3</v>
       </c>
       <c r="C223" s="1" t="s">
-        <v>214</v>
+        <v>156</v>
       </c>
       <c r="D223" s="1" t="s">
         <v>21</v>
@@ -4729,7 +4508,7 @@
         <v>3</v>
       </c>
       <c r="C224" s="1" t="s">
-        <v>217</v>
+        <v>159</v>
       </c>
       <c r="D224" s="1" t="s">
         <v>21</v>
@@ -4743,7 +4522,7 @@
         <v>3</v>
       </c>
       <c r="C225" s="1" t="s">
-        <v>218</v>
+        <v>160</v>
       </c>
       <c r="D225" s="1" t="s">
         <v>21</v>
@@ -4757,7 +4536,7 @@
         <v>12</v>
       </c>
       <c r="C226" s="1" t="s">
-        <v>219</v>
+        <v>161</v>
       </c>
       <c r="D226" s="1" t="s">
         <v>21</v>
@@ -4771,7 +4550,7 @@
         <v>3</v>
       </c>
       <c r="C227" s="1" t="s">
-        <v>220</v>
+        <v>162</v>
       </c>
       <c r="D227" s="1" t="s">
         <v>21</v>
@@ -4785,7 +4564,7 @@
         <v>3</v>
       </c>
       <c r="C228" s="1" t="s">
-        <v>221</v>
+        <v>163</v>
       </c>
       <c r="D228" s="1" t="s">
         <v>21</v>
@@ -4799,7 +4578,7 @@
         <v>3</v>
       </c>
       <c r="C229" s="1" t="s">
-        <v>222</v>
+        <v>164</v>
       </c>
       <c r="D229" s="1" t="s">
         <v>21</v>
@@ -4813,7 +4592,7 @@
         <v>12</v>
       </c>
       <c r="C230" s="1" t="s">
-        <v>223</v>
+        <v>165</v>
       </c>
       <c r="D230" s="1" t="s">
         <v>21</v>
@@ -4841,7 +4620,7 @@
         <v>12</v>
       </c>
       <c r="C232" s="1" t="s">
-        <v>182</v>
+        <v>124</v>
       </c>
       <c r="D232" s="1" t="s">
         <v>21</v>
@@ -4855,7 +4634,7 @@
         <v>3</v>
       </c>
       <c r="C233" s="1" t="s">
-        <v>222</v>
+        <v>164</v>
       </c>
       <c r="D233" s="1" t="s">
         <v>21</v>
@@ -4869,7 +4648,7 @@
         <v>12</v>
       </c>
       <c r="C234" s="1" t="s">
-        <v>223</v>
+        <v>165</v>
       </c>
       <c r="D234" s="1" t="s">
         <v>21</v>
@@ -4897,7 +4676,7 @@
         <v>12</v>
       </c>
       <c r="C236" s="1" t="s">
-        <v>224</v>
+        <v>166</v>
       </c>
       <c r="D236" s="1" t="s">
         <v>21</v>
@@ -4911,7 +4690,7 @@
         <v>3</v>
       </c>
       <c r="C237" s="1" t="s">
-        <v>226</v>
+        <v>168</v>
       </c>
       <c r="D237" s="1" t="s">
         <v>21</v>
@@ -4925,7 +4704,7 @@
         <v>12</v>
       </c>
       <c r="C238" s="1" t="s">
-        <v>225</v>
+        <v>167</v>
       </c>
       <c r="D238" s="1" t="s">
         <v>21</v>
@@ -4939,7 +4718,7 @@
         <v>3</v>
       </c>
       <c r="C239" s="1" t="s">
-        <v>227</v>
+        <v>169</v>
       </c>
       <c r="D239" s="1" t="s">
         <v>21</v>
@@ -4953,7 +4732,7 @@
         <v>12</v>
       </c>
       <c r="C240" s="1" t="s">
-        <v>228</v>
+        <v>170</v>
       </c>
       <c r="D240" s="1" t="s">
         <v>21</v>
@@ -4967,7 +4746,7 @@
         <v>3</v>
       </c>
       <c r="C241" s="1" t="s">
-        <v>229</v>
+        <v>171</v>
       </c>
       <c r="D241" s="1" t="s">
         <v>21</v>
@@ -4981,7 +4760,7 @@
         <v>12</v>
       </c>
       <c r="C242" s="1" t="s">
-        <v>230</v>
+        <v>172</v>
       </c>
       <c r="D242" s="1" t="s">
         <v>21</v>
@@ -4995,7 +4774,7 @@
         <v>3</v>
       </c>
       <c r="C243" s="1" t="s">
-        <v>231</v>
+        <v>173</v>
       </c>
       <c r="D243" s="1" t="s">
         <v>21</v>
@@ -5009,7 +4788,7 @@
         <v>12</v>
       </c>
       <c r="C244" s="1" t="s">
-        <v>232</v>
+        <v>174</v>
       </c>
       <c r="D244" s="1" t="s">
         <v>21</v>
@@ -5023,7 +4802,7 @@
         <v>3</v>
       </c>
       <c r="C245" s="1" t="s">
-        <v>233</v>
+        <v>175</v>
       </c>
       <c r="D245" s="1" t="s">
         <v>21</v>
@@ -5037,7 +4816,7 @@
         <v>12</v>
       </c>
       <c r="C246" s="1" t="s">
-        <v>234</v>
+        <v>176</v>
       </c>
       <c r="D246" s="1" t="s">
         <v>21</v>
@@ -5051,7 +4830,7 @@
         <v>3</v>
       </c>
       <c r="C247" s="1" t="s">
-        <v>235</v>
+        <v>177</v>
       </c>
       <c r="D247" s="1" t="s">
         <v>21</v>
@@ -5065,7 +4844,7 @@
         <v>3</v>
       </c>
       <c r="C248" s="1" t="s">
-        <v>236</v>
+        <v>178</v>
       </c>
       <c r="D248" s="1" t="s">
         <v>21</v>
@@ -5079,7 +4858,7 @@
         <v>12</v>
       </c>
       <c r="C249" s="1" t="s">
-        <v>237</v>
+        <v>179</v>
       </c>
       <c r="D249" s="1" t="s">
         <v>21</v>
@@ -5093,7 +4872,7 @@
         <v>3</v>
       </c>
       <c r="C250" s="1" t="s">
-        <v>239</v>
+        <v>181</v>
       </c>
       <c r="D250" s="1" t="s">
         <v>21</v>
@@ -5107,7 +4886,7 @@
         <v>12</v>
       </c>
       <c r="C251" s="1" t="s">
-        <v>238</v>
+        <v>180</v>
       </c>
       <c r="D251" s="1" t="s">
         <v>21</v>
@@ -5121,7 +4900,7 @@
         <v>3</v>
       </c>
       <c r="C252" s="1" t="s">
-        <v>240</v>
+        <v>182</v>
       </c>
       <c r="D252" s="1" t="s">
         <v>21</v>
@@ -5135,7 +4914,7 @@
         <v>12</v>
       </c>
       <c r="C253" s="1" t="s">
-        <v>241</v>
+        <v>183</v>
       </c>
       <c r="D253" s="1" t="s">
         <v>21</v>
@@ -5149,7 +4928,7 @@
         <v>3</v>
       </c>
       <c r="C254" s="1" t="s">
-        <v>242</v>
+        <v>184</v>
       </c>
       <c r="D254" s="1" t="s">
         <v>21</v>
@@ -5163,7 +4942,7 @@
         <v>3</v>
       </c>
       <c r="C255" s="1" t="s">
-        <v>243</v>
+        <v>185</v>
       </c>
       <c r="D255" s="1" t="s">
         <v>21</v>
@@ -5177,7 +4956,7 @@
         <v>12</v>
       </c>
       <c r="C256" s="1" t="s">
-        <v>176</v>
+        <v>118</v>
       </c>
       <c r="D256" s="1" t="s">
         <v>21</v>
@@ -5191,7 +4970,7 @@
         <v>3</v>
       </c>
       <c r="C257" s="1" t="s">
-        <v>244</v>
+        <v>186</v>
       </c>
       <c r="D257" s="1" t="s">
         <v>21</v>
@@ -5205,7 +4984,7 @@
         <v>3</v>
       </c>
       <c r="C258" s="1" t="s">
-        <v>245</v>
+        <v>187</v>
       </c>
       <c r="D258" s="1" t="s">
         <v>21</v>
@@ -5219,7 +4998,7 @@
         <v>3</v>
       </c>
       <c r="C259" s="1" t="s">
-        <v>246</v>
+        <v>188</v>
       </c>
       <c r="D259" s="1" t="s">
         <v>21</v>
@@ -5233,7 +5012,7 @@
         <v>3</v>
       </c>
       <c r="C260" s="1" t="s">
-        <v>247</v>
+        <v>189</v>
       </c>
       <c r="D260" s="1" t="s">
         <v>21</v>
@@ -5247,7 +5026,7 @@
         <v>3</v>
       </c>
       <c r="C261" s="1" t="s">
-        <v>248</v>
+        <v>190</v>
       </c>
       <c r="D261" s="1" t="s">
         <v>21</v>
@@ -5275,7 +5054,7 @@
         <v>3</v>
       </c>
       <c r="C263" s="1" t="s">
-        <v>249</v>
+        <v>191</v>
       </c>
       <c r="D263" s="1" t="s">
         <v>21</v>
@@ -5289,7 +5068,7 @@
         <v>12</v>
       </c>
       <c r="C264" s="1" t="s">
-        <v>250</v>
+        <v>192</v>
       </c>
       <c r="D264" s="1" t="s">
         <v>21</v>
@@ -5303,7 +5082,7 @@
         <v>3</v>
       </c>
       <c r="C265" s="1" t="s">
-        <v>251</v>
+        <v>193</v>
       </c>
       <c r="D265" s="1" t="s">
         <v>21</v>
@@ -5317,7 +5096,7 @@
         <v>12</v>
       </c>
       <c r="C266" s="1" t="s">
-        <v>252</v>
+        <v>194</v>
       </c>
       <c r="D266" s="1" t="s">
         <v>21</v>
@@ -5331,7 +5110,7 @@
         <v>3</v>
       </c>
       <c r="C267" s="1" t="s">
-        <v>253</v>
+        <v>195</v>
       </c>
       <c r="D267" s="1" t="s">
         <v>21</v>
@@ -5345,7 +5124,7 @@
         <v>12</v>
       </c>
       <c r="C268" s="1" t="s">
-        <v>254</v>
+        <v>196</v>
       </c>
       <c r="D268" s="1" t="s">
         <v>21</v>
@@ -5359,7 +5138,7 @@
         <v>3</v>
       </c>
       <c r="C269" s="1" t="s">
-        <v>255</v>
+        <v>197</v>
       </c>
       <c r="D269" s="1" t="s">
         <v>21</v>
@@ -5373,7 +5152,7 @@
         <v>12</v>
       </c>
       <c r="C270" s="1" t="s">
-        <v>256</v>
+        <v>198</v>
       </c>
       <c r="D270" s="1" t="s">
         <v>21</v>
@@ -5387,7 +5166,7 @@
         <v>3</v>
       </c>
       <c r="C271" s="1" t="s">
-        <v>257</v>
+        <v>199</v>
       </c>
       <c r="D271" s="1" t="s">
         <v>21</v>
@@ -5401,7 +5180,7 @@
         <v>12</v>
       </c>
       <c r="C272" s="1" t="s">
-        <v>258</v>
+        <v>200</v>
       </c>
       <c r="D272" s="1" t="s">
         <v>21</v>
@@ -5415,7 +5194,7 @@
         <v>3</v>
       </c>
       <c r="C273" s="1" t="s">
-        <v>259</v>
+        <v>201</v>
       </c>
       <c r="D273" s="1" t="s">
         <v>21</v>
@@ -5429,7 +5208,7 @@
         <v>12</v>
       </c>
       <c r="C274" s="1" t="s">
-        <v>260</v>
+        <v>202</v>
       </c>
       <c r="D274" s="1" t="s">
         <v>21</v>
@@ -5443,7 +5222,7 @@
         <v>3</v>
       </c>
       <c r="C275" s="1" t="s">
-        <v>262</v>
+        <v>204</v>
       </c>
       <c r="D275" s="1" t="s">
         <v>21</v>
@@ -5457,7 +5236,7 @@
         <v>12</v>
       </c>
       <c r="C276" s="1" t="s">
-        <v>261</v>
+        <v>203</v>
       </c>
       <c r="D276" s="1" t="s">
         <v>21</v>
@@ -5471,7 +5250,7 @@
         <v>3</v>
       </c>
       <c r="C277" s="1" t="s">
-        <v>263</v>
+        <v>205</v>
       </c>
       <c r="D277" s="1" t="s">
         <v>21</v>
@@ -5485,7 +5264,7 @@
         <v>12</v>
       </c>
       <c r="C278" s="1" t="s">
-        <v>264</v>
+        <v>206</v>
       </c>
       <c r="D278" s="1" t="s">
         <v>21</v>
@@ -5499,7 +5278,7 @@
         <v>3</v>
       </c>
       <c r="C279" s="1" t="s">
-        <v>149</v>
+        <v>91</v>
       </c>
       <c r="D279" s="1" t="s">
         <v>21</v>
@@ -5513,7 +5292,7 @@
         <v>3</v>
       </c>
       <c r="C280" s="1" t="s">
-        <v>265</v>
+        <v>207</v>
       </c>
       <c r="D280" s="1" t="s">
         <v>21</v>
@@ -5527,7 +5306,7 @@
         <v>12</v>
       </c>
       <c r="C281" s="1" t="s">
-        <v>266</v>
+        <v>208</v>
       </c>
       <c r="D281" s="1" t="s">
         <v>21</v>
@@ -5541,7 +5320,7 @@
         <v>3</v>
       </c>
       <c r="C282" s="1" t="s">
-        <v>268</v>
+        <v>210</v>
       </c>
       <c r="D282" s="1" t="s">
         <v>21</v>
@@ -5555,7 +5334,7 @@
         <v>12</v>
       </c>
       <c r="C283" s="1" t="s">
-        <v>267</v>
+        <v>209</v>
       </c>
       <c r="D283" s="1" t="s">
         <v>21</v>
@@ -5569,7 +5348,7 @@
         <v>3</v>
       </c>
       <c r="C284" s="1" t="s">
-        <v>269</v>
+        <v>211</v>
       </c>
       <c r="D284" s="1" t="s">
         <v>21</v>
@@ -5583,7 +5362,7 @@
         <v>12</v>
       </c>
       <c r="C285" s="1" t="s">
-        <v>270</v>
+        <v>212</v>
       </c>
       <c r="D285" s="1" t="s">
         <v>21</v>
@@ -5597,7 +5376,7 @@
         <v>3</v>
       </c>
       <c r="C286" s="1" t="s">
-        <v>272</v>
+        <v>214</v>
       </c>
       <c r="D286" s="1" t="s">
         <v>21</v>
@@ -5611,7 +5390,7 @@
         <v>12</v>
       </c>
       <c r="C287" s="1" t="s">
-        <v>271</v>
+        <v>213</v>
       </c>
       <c r="D287" s="1" t="s">
         <v>21</v>
@@ -5625,7 +5404,7 @@
         <v>3</v>
       </c>
       <c r="C288" s="1" t="s">
-        <v>273</v>
+        <v>215</v>
       </c>
       <c r="D288" s="1" t="s">
         <v>21</v>
@@ -5639,7 +5418,7 @@
         <v>12</v>
       </c>
       <c r="C289" s="1" t="s">
-        <v>274</v>
+        <v>216</v>
       </c>
       <c r="D289" s="1" t="s">
         <v>21</v>
@@ -5653,7 +5432,7 @@
         <v>3</v>
       </c>
       <c r="C290" s="1" t="s">
-        <v>275</v>
+        <v>217</v>
       </c>
       <c r="D290" s="1" t="s">
         <v>21</v>
@@ -5667,7 +5446,7 @@
         <v>12</v>
       </c>
       <c r="C291" s="1" t="s">
-        <v>276</v>
+        <v>218</v>
       </c>
       <c r="D291" s="1" t="s">
         <v>21</v>
@@ -5681,7 +5460,7 @@
         <v>3</v>
       </c>
       <c r="C292" s="1" t="s">
-        <v>277</v>
+        <v>219</v>
       </c>
       <c r="D292" s="1" t="s">
         <v>21</v>
@@ -5695,7 +5474,7 @@
         <v>12</v>
       </c>
       <c r="C293" s="1" t="s">
-        <v>278</v>
+        <v>220</v>
       </c>
       <c r="D293" s="1" t="s">
         <v>21</v>
@@ -5709,7 +5488,7 @@
         <v>3</v>
       </c>
       <c r="C294" s="1" t="s">
-        <v>279</v>
+        <v>221</v>
       </c>
       <c r="D294" s="1" t="s">
         <v>21</v>
@@ -5723,7 +5502,7 @@
         <v>12</v>
       </c>
       <c r="C295" s="1" t="s">
-        <v>280</v>
+        <v>222</v>
       </c>
       <c r="D295" s="1" t="s">
         <v>21</v>
@@ -5737,7 +5516,7 @@
         <v>3</v>
       </c>
       <c r="C296" s="1" t="s">
-        <v>281</v>
+        <v>223</v>
       </c>
       <c r="D296" s="1" t="s">
         <v>21</v>
@@ -5751,7 +5530,7 @@
         <v>12</v>
       </c>
       <c r="C297" s="1" t="s">
-        <v>282</v>
+        <v>224</v>
       </c>
       <c r="D297" s="1" t="s">
         <v>21</v>
@@ -5765,7 +5544,7 @@
         <v>3</v>
       </c>
       <c r="C298" s="1" t="s">
-        <v>283</v>
+        <v>225</v>
       </c>
       <c r="D298" s="1" t="s">
         <v>21</v>
@@ -5779,7 +5558,7 @@
         <v>12</v>
       </c>
       <c r="C299" s="1" t="s">
-        <v>284</v>
+        <v>226</v>
       </c>
       <c r="D299" s="1" t="s">
         <v>21</v>
@@ -5793,7 +5572,7 @@
         <v>3</v>
       </c>
       <c r="C300" s="1" t="s">
-        <v>286</v>
+        <v>228</v>
       </c>
       <c r="D300" s="1" t="s">
         <v>21</v>
@@ -5807,7 +5586,7 @@
         <v>12</v>
       </c>
       <c r="C301" s="1" t="s">
-        <v>285</v>
+        <v>227</v>
       </c>
       <c r="D301" s="1" t="s">
         <v>21</v>
@@ -5821,7 +5600,7 @@
         <v>3</v>
       </c>
       <c r="C302" s="1" t="s">
-        <v>287</v>
+        <v>229</v>
       </c>
       <c r="D302" s="1" t="s">
         <v>21</v>
@@ -5835,7 +5614,7 @@
         <v>12</v>
       </c>
       <c r="C303" s="1" t="s">
-        <v>288</v>
+        <v>230</v>
       </c>
       <c r="D303" s="1" t="s">
         <v>21</v>
@@ -5849,7 +5628,7 @@
         <v>3</v>
       </c>
       <c r="C304" s="1" t="s">
-        <v>290</v>
+        <v>232</v>
       </c>
       <c r="D304" s="1" t="s">
         <v>21</v>
@@ -5863,7 +5642,7 @@
         <v>12</v>
       </c>
       <c r="C305" s="1" t="s">
-        <v>289</v>
+        <v>231</v>
       </c>
       <c r="D305" s="1" t="s">
         <v>21</v>
@@ -5877,7 +5656,7 @@
         <v>3</v>
       </c>
       <c r="C306" s="1" t="s">
-        <v>291</v>
+        <v>233</v>
       </c>
       <c r="D306" s="1" t="s">
         <v>21</v>
@@ -5891,7 +5670,7 @@
         <v>12</v>
       </c>
       <c r="C307" s="1" t="s">
-        <v>292</v>
+        <v>234</v>
       </c>
       <c r="D307" s="1" t="s">
         <v>21</v>
@@ -5905,7 +5684,7 @@
         <v>3</v>
       </c>
       <c r="C308" s="1" t="s">
-        <v>293</v>
+        <v>235</v>
       </c>
       <c r="D308" s="1" t="s">
         <v>21</v>
@@ -5919,7 +5698,7 @@
         <v>12</v>
       </c>
       <c r="C309" s="1" t="s">
-        <v>294</v>
+        <v>236</v>
       </c>
       <c r="D309" s="1" t="s">
         <v>21</v>
@@ -5933,7 +5712,7 @@
         <v>3</v>
       </c>
       <c r="C310" s="1" t="s">
-        <v>53</v>
+        <v>24</v>
       </c>
       <c r="D310" s="1" t="s">
         <v>21</v>
@@ -5947,7 +5726,7 @@
         <v>12</v>
       </c>
       <c r="C311" s="1" t="s">
-        <v>182</v>
+        <v>124</v>
       </c>
       <c r="D311" s="1" t="s">
         <v>21</v>
@@ -5961,7 +5740,7 @@
         <v>3</v>
       </c>
       <c r="C312" s="1" t="s">
-        <v>295</v>
+        <v>237</v>
       </c>
       <c r="D312" s="1" t="s">
         <v>21</v>
@@ -5975,7 +5754,7 @@
         <v>12</v>
       </c>
       <c r="C313" s="1" t="s">
-        <v>296</v>
+        <v>238</v>
       </c>
       <c r="D313" s="1" t="s">
         <v>21</v>
@@ -5989,7 +5768,7 @@
         <v>3</v>
       </c>
       <c r="C314" s="1" t="s">
-        <v>297</v>
+        <v>239</v>
       </c>
       <c r="D314" s="1" t="s">
         <v>21</v>
@@ -6003,7 +5782,7 @@
         <v>12</v>
       </c>
       <c r="C315" s="1" t="s">
-        <v>298</v>
+        <v>240</v>
       </c>
       <c r="D315" s="1" t="s">
         <v>21</v>
@@ -6017,7 +5796,7 @@
         <v>3</v>
       </c>
       <c r="C316" s="1" t="s">
-        <v>299</v>
+        <v>241</v>
       </c>
       <c r="D316" s="1" t="s">
         <v>21</v>
@@ -6031,7 +5810,7 @@
         <v>12</v>
       </c>
       <c r="C317" s="1" t="s">
-        <v>300</v>
+        <v>242</v>
       </c>
       <c r="D317" s="1" t="s">
         <v>21</v>
@@ -6045,7 +5824,7 @@
         <v>12</v>
       </c>
       <c r="C318" s="1" t="s">
-        <v>301</v>
+        <v>243</v>
       </c>
       <c r="D318" s="1" t="s">
         <v>21</v>
@@ -6059,7 +5838,7 @@
         <v>3</v>
       </c>
       <c r="C319" s="1" t="s">
-        <v>172</v>
+        <v>114</v>
       </c>
       <c r="D319" s="1" t="s">
         <v>21</v>
@@ -6073,7 +5852,7 @@
         <v>12</v>
       </c>
       <c r="C320" s="1" t="s">
-        <v>302</v>
+        <v>244</v>
       </c>
       <c r="D320" s="1" t="s">
         <v>21</v>
@@ -6087,7 +5866,7 @@
         <v>3</v>
       </c>
       <c r="C321" s="1" t="s">
-        <v>303</v>
+        <v>245</v>
       </c>
       <c r="D321" s="1" t="s">
         <v>21</v>
@@ -6101,7 +5880,7 @@
         <v>12</v>
       </c>
       <c r="C322" s="1" t="s">
-        <v>304</v>
+        <v>246</v>
       </c>
       <c r="D322" s="1" t="s">
         <v>21</v>
@@ -6115,7 +5894,7 @@
         <v>3</v>
       </c>
       <c r="C323" s="1" t="s">
-        <v>305</v>
+        <v>247</v>
       </c>
       <c r="D323" s="1" t="s">
         <v>21</v>
@@ -6129,7 +5908,7 @@
         <v>12</v>
       </c>
       <c r="C324" s="1" t="s">
-        <v>306</v>
+        <v>248</v>
       </c>
       <c r="D324" s="1" t="s">
         <v>21</v>
@@ -6143,7 +5922,7 @@
         <v>12</v>
       </c>
       <c r="C325" s="1" t="s">
-        <v>307</v>
+        <v>249</v>
       </c>
       <c r="D325" s="1" t="s">
         <v>21</v>
@@ -6157,7 +5936,7 @@
         <v>3</v>
       </c>
       <c r="C326" s="1" t="s">
-        <v>308</v>
+        <v>250</v>
       </c>
       <c r="D326" s="1" t="s">
         <v>21</v>
@@ -6171,7 +5950,7 @@
         <v>12</v>
       </c>
       <c r="C327" s="1" t="s">
-        <v>309</v>
+        <v>251</v>
       </c>
       <c r="D327" s="1" t="s">
         <v>21</v>
@@ -6185,7 +5964,7 @@
         <v>3</v>
       </c>
       <c r="C328" s="1" t="s">
-        <v>243</v>
+        <v>185</v>
       </c>
       <c r="D328" s="1" t="s">
         <v>21</v>
@@ -6199,7 +5978,7 @@
         <v>12</v>
       </c>
       <c r="C329" s="1" t="s">
-        <v>310</v>
+        <v>252</v>
       </c>
       <c r="D329" s="1" t="s">
         <v>21</v>
@@ -6227,7 +6006,7 @@
         <v>12</v>
       </c>
       <c r="C331" s="1" t="s">
-        <v>179</v>
+        <v>121</v>
       </c>
       <c r="D331" s="1" t="s">
         <v>21</v>
@@ -6241,7 +6020,7 @@
         <v>3</v>
       </c>
       <c r="C332" s="1" t="s">
-        <v>257</v>
+        <v>199</v>
       </c>
       <c r="D332" s="1" t="s">
         <v>21</v>
@@ -6255,7 +6034,7 @@
         <v>12</v>
       </c>
       <c r="C333" s="1" t="s">
-        <v>258</v>
+        <v>200</v>
       </c>
       <c r="D333" s="1" t="s">
         <v>21</v>
@@ -6269,7 +6048,7 @@
         <v>3</v>
       </c>
       <c r="C334" s="1" t="s">
-        <v>311</v>
+        <v>253</v>
       </c>
       <c r="D334" s="1" t="s">
         <v>21</v>
@@ -6283,7 +6062,7 @@
         <v>12</v>
       </c>
       <c r="C335" s="1" t="s">
-        <v>312</v>
+        <v>254</v>
       </c>
       <c r="D335" s="1" t="s">
         <v>21</v>
@@ -6297,7 +6076,7 @@
         <v>3</v>
       </c>
       <c r="C336" s="1" t="s">
-        <v>313</v>
+        <v>255</v>
       </c>
       <c r="D336" s="1" t="s">
         <v>21</v>
@@ -6311,7 +6090,7 @@
         <v>3</v>
       </c>
       <c r="C337" s="1" t="s">
-        <v>315</v>
+        <v>257</v>
       </c>
       <c r="D337" s="1" t="s">
         <v>21</v>
@@ -6325,7 +6104,7 @@
         <v>12</v>
       </c>
       <c r="C338" s="1" t="s">
-        <v>314</v>
+        <v>256</v>
       </c>
       <c r="D338" s="1" t="s">
         <v>21</v>
@@ -6339,7 +6118,7 @@
         <v>3</v>
       </c>
       <c r="C339" s="1" t="s">
-        <v>316</v>
+        <v>258</v>
       </c>
       <c r="D339" s="1" t="s">
         <v>21</v>
@@ -6353,7 +6132,7 @@
         <v>3</v>
       </c>
       <c r="C340" s="1" t="s">
-        <v>317</v>
+        <v>259</v>
       </c>
       <c r="D340" s="1" t="s">
         <v>21</v>
@@ -6367,7 +6146,7 @@
         <v>3</v>
       </c>
       <c r="C341" s="1" t="s">
-        <v>318</v>
+        <v>260</v>
       </c>
       <c r="D341" s="1" t="s">
         <v>21</v>
@@ -6381,7 +6160,7 @@
         <v>12</v>
       </c>
       <c r="C342" s="1" t="s">
-        <v>319</v>
+        <v>261</v>
       </c>
       <c r="D342" s="1" t="s">
         <v>21</v>
@@ -6395,7 +6174,7 @@
         <v>3</v>
       </c>
       <c r="C343" s="1" t="s">
-        <v>320</v>
+        <v>262</v>
       </c>
       <c r="D343" s="1" t="s">
         <v>21</v>
@@ -6409,7 +6188,7 @@
         <v>12</v>
       </c>
       <c r="C344" s="1" t="s">
-        <v>321</v>
+        <v>263</v>
       </c>
       <c r="D344" s="1" t="s">
         <v>21</v>
@@ -6423,7 +6202,7 @@
         <v>3</v>
       </c>
       <c r="C345" s="1" t="s">
-        <v>54</v>
+        <v>25</v>
       </c>
       <c r="D345" s="1" t="s">
         <v>21</v>
@@ -6451,7 +6230,7 @@
         <v>3</v>
       </c>
       <c r="C347" s="1" t="s">
-        <v>322</v>
+        <v>264</v>
       </c>
       <c r="D347" s="1" t="s">
         <v>21</v>
@@ -6465,7 +6244,7 @@
         <v>3</v>
       </c>
       <c r="C348" s="1" t="s">
-        <v>323</v>
+        <v>265</v>
       </c>
       <c r="D348" s="1" t="s">
         <v>21</v>
@@ -6483,7 +6262,7 @@
       <formula>NOT(ISERROR(SEARCH("ADICIONAR",D1)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B1:B139 B140:C140 C141:C145 C147:C151 B141:B1048576">
+  <conditionalFormatting sqref="B140:C140 C141:C145 C147:C151 B141:B1048576 B1:B139">
     <cfRule type="containsText" dxfId="2" priority="1" operator="containsText" text="pt">
       <formula>NOT(ISERROR(SEARCH("pt",B1)))</formula>
     </cfRule>

</xml_diff>